<commit_message>
doc in progress ...
</commit_message>
<xml_diff>
--- a/doc/contents.xlsx
+++ b/doc/contents.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="460" windowWidth="19660" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="5860" yWindow="460" windowWidth="19660" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="98">
   <si>
     <t>task</t>
   </si>
@@ -48,9 +48,6 @@
     <t>input</t>
   </si>
   <si>
-    <t>Enter Data</t>
-  </si>
-  <si>
     <t>pandas</t>
   </si>
   <si>
@@ -522,9 +519,6 @@
   </si>
   <si>
     <t>feature representation</t>
-  </si>
-  <si>
-    <t>Define Model</t>
   </si>
   <si>
     <t>regression</t>
@@ -582,9 +576,6 @@
   </si>
   <si>
     <t>:py:func:`cheml.initialization.SaveFile`</t>
-  </si>
-  <si>
-    <t>filename = required for the function</t>
   </si>
   <si>
     <r>
@@ -647,6 +638,18 @@
     <t>version = 6,CheckUpdates = True,SaveLayout = True, PreserveTemporaryProjects = True, ShowWorksheet = False,Decimal_Separator = ".",Missing_String = "NaN",DefaultMolFormat = "1",HelpBrowser = "/usr/bin/xdg-open",RejectUnusualValence = False,Add2DHydrogens = False,MaxSRforAllCircuit = "19",MaxSR = "35",MaxSRDetour = "30",MaxAtomWalkPath = "2000",LogPathWalk = True,LogEdge = True,Weights = ["Mass"-"VdWVolume"-"Electronegativity"-"Polarizability"-"Ionization"-"I-State"],SaveOnlyData = False,SaveLabelsOnSeparateFile = False,SaveFormatBlock = "%b-%n.txt",SaveFormatSubBlock = "%b-%s-%n-%m.txt",SaveExcludeMisVal = False,SaveExcludeAllMisVal = False,SaveExcludeConst = False,SaveExcludeNearConst = False,SaveExcludeStdDev = False,SaveStdDevThreshold = "0.0001",SaveExcludeCorrelated = False,SaveCorrThreshold = "0.95",
                 SaveExclusionOptionsToVariables = False,SaveExcludeMisMolecules = False,
 SaveExcludeRejectedMolecules = False,blocks = range(1-30),molInput = "stdin",molInputFormat = "SMILES",molFile = None,SaveStdOut = False,SaveProject = False,SaveProjectFile = "Dragon_project.drp",SaveFile = True,SaveType = "singlefile", SaveFilePath = "Dragon_descriptors.txt",logMode = "file",logFile = "Dragon_log.txt",external = False,fileName = None,delimiter = "-",consecutiveDelimiter = False,MissingValue = "NaN", RejectDisconnectedStrucuture = False, RetainBiggestFragment = False, DisconnectedCalculationOption = "0",RoundCoordinates = True, RoundWeights = True, RoundDescriptorValues = True, knimemode = False</t>
+  </si>
+  <si>
+    <t>filename = : required for the function</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Prepare</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1113,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,22 +1141,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1161,34 +1164,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1196,34 +1199,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1231,34 +1234,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1266,34 +1269,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1301,34 +1304,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
         <v>61</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>63</v>
       </c>
-      <c r="I6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" t="s">
-        <v>64</v>
-      </c>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1336,34 +1339,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" t="s">
-        <v>61</v>
-      </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1371,34 +1374,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="G8" t="s">
-        <v>61</v>
-      </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1406,34 +1409,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1441,34 +1444,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" t="s">
-        <v>40</v>
-      </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1476,34 +1479,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
         <v>68</v>
       </c>
-      <c r="H11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>69</v>
-      </c>
-      <c r="K11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1511,34 +1514,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>73</v>
-      </c>
-      <c r="K12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1546,34 +1549,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1581,34 +1584,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" t="s">
-        <v>77</v>
-      </c>
       <c r="K14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1616,34 +1619,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1651,34 +1654,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="H16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="J16" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J16" t="s">
-        <v>87</v>
-      </c>
       <c r="K16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1686,34 +1689,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
         <v>89</v>
       </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" t="s">
-        <v>92</v>
-      </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1732,22 +1735,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1773,26 +1776,26 @@
   <sheetData>
     <row r="1" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>